<commit_message>
Creating a folder. Newest version after first UAT/monitored live run
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RPA\Processes\NewDawnFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aevesbv-my.sharepoint.com/personal/sbeukema_newdawnrobotics_nl/Documents/Documenten/UiPath/NDR_Orchestrator_CreateFolder/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53668DA9-7F9E-4609-AF82-7EDEA5229582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{53668DA9-7F9E-4609-AF82-7EDEA5229582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01A85DFD-4623-4243-9A65-67375169554A}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>NewDawnRobotics</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <r>
@@ -311,9 +308,6 @@
     <t>The number of times Dispatcher is retried in case of an exceptoin. Must be an integer &gt;=1.</t>
   </si>
   <si>
-    <t>RPAXXX</t>
-  </si>
-  <si>
     <t>The name of the customer.</t>
   </si>
   <si>
@@ -372,12 +366,27 @@
   <si>
     <t>OrchestratorAssetFolderProd</t>
   </si>
+  <si>
+    <t>RPA002</t>
+  </si>
+  <si>
+    <t>Orchestrator_CreateFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorCloudPrefix</t>
+  </si>
+  <si>
+    <t>https://cloud.uipath.com/newdawnrobotics/{0}/orchestrator_/</t>
+  </si>
+  <si>
+    <t>Base of the Cloud URL. Replace the {0} for the tenant name in the robot</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -388,6 +397,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -432,6 +442,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -445,6 +456,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -513,10 +532,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -576,9 +596,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -630,9 +652,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -670,7 +692,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -776,7 +798,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -918,7 +940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -928,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1019"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -998,7 +1020,7 @@
         <v>NewDawnRobotics</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
@@ -1006,14 +1028,14 @@
         <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C5" s="16" t="str">
         <f>B5</f>
-        <v>RPAXXX</v>
+        <v>RPA002</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
@@ -1021,20 +1043,20 @@
         <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C6" s="16" t="str">
         <f>B6</f>
-        <v>Framework</v>
+        <v>Orchestrator_CreateFolder</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="13.9" customHeight="1"/>
     <row r="8" spans="1:27" ht="13.9" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -1042,89 +1064,89 @@
     </row>
     <row r="9" spans="1:27" ht="30" customHeight="1">
       <c r="A9" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B9" s="20" t="str">
         <f>"C:\RPA\Test\"&amp;B17</f>
-        <v>C:\RPA\Test\NewDawnRobotics_RPAXXX_Framework</v>
+        <v>C:\RPA\Test\NewDawnRobotics_RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="C9" s="20" t="str">
         <f>"C:\RPA\"&amp;C17</f>
-        <v>C:\RPA\NewDawnRobotics_RPAXXX_Framework</v>
+        <v>C:\RPA\NewDawnRobotics_RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="13.9" customHeight="1">
       <c r="A10" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="20" t="str">
         <f>B$9&amp;"\Input"</f>
-        <v>C:\RPA\Test\NewDawnRobotics_RPAXXX_Framework\Input</v>
+        <v>C:\RPA\Test\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Input</v>
       </c>
       <c r="C10" s="20" t="str">
         <f>C$9&amp;"\Input"</f>
-        <v>C:\RPA\NewDawnRobotics_RPAXXX_Framework\Input</v>
+        <v>C:\RPA\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Input</v>
       </c>
       <c r="D10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="13.9" customHeight="1">
       <c r="A11" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B11" s="20" t="str">
         <f>B$9&amp;"\Temp"</f>
-        <v>C:\RPA\Test\NewDawnRobotics_RPAXXX_Framework\Temp</v>
+        <v>C:\RPA\Test\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Temp</v>
       </c>
       <c r="C11" s="20" t="str">
         <f>C$9&amp;"\Temp"</f>
-        <v>C:\RPA\NewDawnRobotics_RPAXXX_Framework\Temp</v>
+        <v>C:\RPA\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Temp</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="13.9" customHeight="1">
       <c r="A12" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B12" s="20" t="str">
         <f>B$9&amp;"\Output"</f>
-        <v>C:\RPA\Test\NewDawnRobotics_RPAXXX_Framework\Output</v>
+        <v>C:\RPA\Test\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Output</v>
       </c>
       <c r="C12" s="20" t="str">
         <f>C$9&amp;"\Output"</f>
-        <v>C:\RPA\NewDawnRobotics_RPAXXX_Framework\Output</v>
+        <v>C:\RPA\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Output</v>
       </c>
       <c r="D12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="13.9" customHeight="1">
       <c r="A13" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="20" t="str">
         <f>B$9&amp;"\Exception_Screenshots"</f>
-        <v>C:\RPA\Test\NewDawnRobotics_RPAXXX_Framework\Exception_Screenshots</v>
+        <v>C:\RPA\Test\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Exception_Screenshots</v>
       </c>
       <c r="C13" s="20" t="str">
         <f>C$9&amp;"\Exception_Screenshots"</f>
-        <v>C:\RPA\NewDawnRobotics_RPAXXX_Framework\Exception_Screenshots</v>
+        <v>C:\RPA\NewDawnRobotics_RPA002_Orchestrator_CreateFolder\Exception_Screenshots</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="13.9" customHeight="1"/>
     <row r="15" spans="1:27" ht="13.9" customHeight="1"/>
     <row r="16" spans="1:27" ht="14.25" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1136,14 +1158,14 @@
       </c>
       <c r="B17" s="16" t="str">
         <f>B$4&amp;"_"&amp;B$5&amp;"_"&amp;B$6</f>
-        <v>NewDawnRobotics_RPAXXX_Framework</v>
+        <v>NewDawnRobotics_RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="C17" s="16" t="str">
         <f>C$4&amp;"_"&amp;C$5&amp;"_"&amp;C$6</f>
-        <v>NewDawnRobotics_RPAXXX_Framework</v>
+        <v>NewDawnRobotics_RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45">
@@ -1152,14 +1174,14 @@
       </c>
       <c r="B18" s="16" t="str">
         <f>B$5&amp;"_"&amp;B$6</f>
-        <v>RPAXXX_Framework</v>
+        <v>RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="C18" s="16" t="str">
         <f>C$5&amp;"_"&amp;C$6</f>
-        <v>RPAXXX_Framework</v>
+        <v>RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30">
@@ -1168,30 +1190,30 @@
       </c>
       <c r="B19" s="16" t="str">
         <f>B$5&amp;"_"&amp;B$6</f>
-        <v>RPAXXX_Framework</v>
+        <v>RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="C19" s="16" t="str">
         <f>C$5&amp;"_"&amp;C$6</f>
-        <v>RPAXXX_Framework</v>
+        <v>RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30">
       <c r="A20" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="16" t="str">
         <f>B$5&amp;"_"&amp;B$6&amp;"_Reporter"</f>
-        <v>RPAXXX_Framework_Reporter</v>
+        <v>RPA002_Orchestrator_CreateFolder_Reporter</v>
       </c>
       <c r="C20" s="16" t="str">
         <f>C$5&amp;"_"&amp;C$6&amp;"_Reporter"</f>
-        <v>RPAXXX_Framework_Reporter</v>
+        <v>RPA002_Orchestrator_CreateFolder_Reporter</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30">
@@ -1200,14 +1222,14 @@
       </c>
       <c r="B21" s="16" t="str">
         <f>B$17</f>
-        <v>NewDawnRobotics_RPAXXX_Framework</v>
+        <v>NewDawnRobotics_RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="C21" s="16" t="str">
         <f>C$17</f>
-        <v>NewDawnRobotics_RPAXXX_Framework</v>
+        <v>NewDawnRobotics_RPA002_Orchestrator_CreateFolder</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30">
@@ -1221,7 +1243,7 @@
         <v>6</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1232,7 +1254,7 @@
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1">
       <c r="A25" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
@@ -1249,13 +1271,26 @@
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1">
       <c r="A29" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="14"/>
       <c r="C29" s="14"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -2272,8 +2307,12 @@
       <formula>IF($C9&lt;&gt;"",$C9&lt;&gt;$B9,"")</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="B30" r:id="rId1" xr:uid="{719354D6-26BA-47D0-8682-35C27110EED6}"/>
+    <hyperlink ref="C30" r:id="rId2" xr:uid="{F67A32FD-A5DD-4E2E-9E03-FB4461527E77}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2281,7 +2320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2460,7 +2499,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3476,10 +3515,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -4538,7 +4577,7 @@
     </row>
     <row r="2" spans="1:3" ht="120">
       <c r="A2" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>34</v>

</xml_diff>